<commit_message>
added multithreading to aws.py and main.py added .gif extension to landing_page_details.json
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/013.xlsx
+++ b/docs/STAFF-DATA/013.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15418400-0D77-4CD1-9245-26F17A27EBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25525BD6-16AD-49BB-AED5-1C14DE13C4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,9 +451,6 @@
     <t>VEC-013-05-015</t>
   </si>
   <si>
-    <t>/static/images/principal_data/VEC-013-02-200.webp</t>
-  </si>
-  <si>
     <t>Mr. PRASAD J</t>
   </si>
   <si>
@@ -464,6 +461,9 @@
   </si>
   <si>
     <t>Mr. ARUMUGAM B</t>
+  </si>
+  <si>
+    <t>/static/images/profile_photos/013/VEC-013-02-200.webp</t>
   </si>
 </sst>
 </file>
@@ -861,7 +861,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,7 +943,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="20" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
         <v>133</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="21" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
         <v>136</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="22" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
         <v>133</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="23" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" t="s">
         <v>133</v>

</xml_diff>